<commit_message>
Game save. Successful connection to xArm as HidDevice under UWP.
</commit_message>
<xml_diff>
--- a/VS/LewanSoul-xArm/USB Commands.xlsx
+++ b/VS/LewanSoul-xArm/USB Commands.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC22024-B969-45E7-A353-8F3F6720C244}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,97 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+  <si>
+    <t>xArm App MainWindow.cs</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>CMD_MULT_SERVO_MOVE</t>
+  </si>
+  <si>
+    <t>CMD_ACTION_DOWNLOAD</t>
+  </si>
+  <si>
+    <t>CMD_FULL_ACTION_RUN</t>
+  </si>
+  <si>
+    <t>CMD_FULL_ACTION_STOP</t>
+  </si>
+  <si>
+    <t>CMD_FULL_ACTION_ERASE</t>
+  </si>
+  <si>
+    <t>CMD_SERVO_OFFSET_WRITE</t>
+  </si>
+  <si>
+    <t>CMD_SERVO_OFFSET_READ</t>
+  </si>
+  <si>
+    <t>CMD_SERVO_OFFSET_ADJUST</t>
+  </si>
+  <si>
+    <t>CMD_MULT_SERVO_UNLOAD</t>
+  </si>
+  <si>
+    <t>CMD_MULT_SERVO_POS_READ</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_OFFSET_WRITE</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_OFFSET_READ</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_OFFSET_ADJUST</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_MOROR_CTRL</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_INFO_WRITE</t>
+  </si>
+  <si>
+    <t>CMD_BUS_SERVO_INFO_READ</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Command Format</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Data Length</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>0x55 0x55</t>
+  </si>
+  <si>
+    <t>Cmd</t>
+  </si>
+  <si>
+    <t>Prm 1…Prm N</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +420,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>